<commit_message>
Change the Config File Data - (5-27-2025)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive\Documents\UiPath\UiPath_RPA_Challenge\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F4CA4A-4623-46B4-A8E6-04CEE1F4F269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966B25D7-5B75-4A48-803F-1F782DBEA992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22932" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -168,22 +168,25 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>These apps will be close befor run the automation. If there any brouses that need to kill befor process run add here</t>
-  </si>
-  <si>
     <t>WebsiteLink</t>
   </si>
   <si>
     <t>https://rpachallenge.com/</t>
   </si>
   <si>
-    <t>indicate using which broser you needed to do the developmet. Chrome /msedge</t>
-  </si>
-  <si>
     <t>chrome</t>
   </si>
   <si>
     <t>chrome,excel</t>
+  </si>
+  <si>
+    <t>These applications will be closed before the automation starts. Add any other apps here if they need to be killed before execution.</t>
+  </si>
+  <si>
+    <t>Indicates which browser to use for automation. Supports 'chrome' or 'msedge'.</t>
+  </si>
+  <si>
+    <t>The URL of the RPA Challenge site</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -645,10 +648,10 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -656,18 +659,21 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>49</v>
+      <c r="C8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>